<commit_message>
feat: add filter funcs
</commit_message>
<xml_diff>
--- a/src/assets/notneed.xlsx
+++ b/src/assets/notneed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leo/workspace/other-projects/pcauto-crawler/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\workspace\other-projects\pcauto-crawler\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB5E7217-EFB7-2744-AF86-11AD52B2477C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C220E55E-F4A4-4A90-9F2D-E2CAB67A5502}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11480" yWindow="5460" windowWidth="28240" windowHeight="17440" xr2:uid="{9D75F08C-35DA-3842-9882-0D06AC8566A7}"/>
+    <workbookView xWindow="11475" yWindow="5460" windowWidth="28245" windowHeight="17445" xr2:uid="{9D75F08C-35DA-3842-9882-0D06AC8566A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
   <si>
     <t>notneed</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -35,13 +35,304 @@
   </si>
   <si>
     <t>阿尔法·罗密欧</t>
+  </si>
+  <si>
+    <t>AC Schnitzer</t>
+  </si>
+  <si>
+    <t>艾康尼克</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALPINA</t>
+  </si>
+  <si>
+    <t>爱驰</t>
+  </si>
+  <si>
+    <t>Arash</t>
+  </si>
+  <si>
+    <t>布加迪</t>
+  </si>
+  <si>
+    <t>巴博斯</t>
+  </si>
+  <si>
+    <t>BYTON</t>
+  </si>
+  <si>
+    <t>成功</t>
+  </si>
+  <si>
+    <t>刺猬汽车</t>
+  </si>
+  <si>
+    <t>CUPRA</t>
+  </si>
+  <si>
+    <t>昶洧</t>
+  </si>
+  <si>
+    <t>大发</t>
+  </si>
+  <si>
+    <t>大迪</t>
+  </si>
+  <si>
+    <t>东风瑞泰特</t>
+  </si>
+  <si>
+    <t>Dacia</t>
+  </si>
+  <si>
+    <t>Fisker</t>
+  </si>
+  <si>
+    <t>FM Auto</t>
+  </si>
+  <si>
+    <t>光冈</t>
+  </si>
+  <si>
+    <t>合众新能源</t>
+  </si>
+  <si>
+    <t>海格</t>
+  </si>
+  <si>
+    <t>华普</t>
+  </si>
+  <si>
+    <t>红星</t>
+  </si>
+  <si>
+    <t>恒天</t>
+  </si>
+  <si>
+    <t>合众汽车</t>
+  </si>
+  <si>
+    <t>Hennessey</t>
+  </si>
+  <si>
+    <t>ITALDESIGN</t>
+  </si>
+  <si>
+    <t>Isdera</t>
+  </si>
+  <si>
+    <t>捷途</t>
+  </si>
+  <si>
+    <t>君马汽车</t>
+  </si>
+  <si>
+    <t>金龙汽车</t>
+  </si>
+  <si>
+    <t>金旅</t>
+  </si>
+  <si>
+    <t>奇点汽车</t>
+  </si>
+  <si>
+    <t>开瑞</t>
+  </si>
+  <si>
+    <t>科尼赛克</t>
+  </si>
+  <si>
+    <t>卡威汽车</t>
+  </si>
+  <si>
+    <t>卡升</t>
+  </si>
+  <si>
+    <t>KTM</t>
+  </si>
+  <si>
+    <t>凯马</t>
+  </si>
+  <si>
+    <t>科瑞斯的</t>
+  </si>
+  <si>
+    <t>兰博基尼</t>
+  </si>
+  <si>
+    <t>劳斯莱斯</t>
+  </si>
+  <si>
+    <t>路特斯</t>
+  </si>
+  <si>
+    <t>理想智造</t>
+  </si>
+  <si>
+    <t>雷丁</t>
+  </si>
+  <si>
+    <t>零跑</t>
+  </si>
+  <si>
+    <t>莲花</t>
+  </si>
+  <si>
+    <t>Lorinser</t>
+  </si>
+  <si>
+    <t>LOCAL MOTORS</t>
+  </si>
+  <si>
+    <t>领途</t>
+  </si>
+  <si>
+    <t>拉达</t>
+  </si>
+  <si>
+    <t>LeSEE</t>
+  </si>
+  <si>
+    <t>朗世</t>
+  </si>
+  <si>
+    <t>拉共达</t>
+  </si>
+  <si>
+    <t>Lucid</t>
+  </si>
+  <si>
+    <t>玛莎拉蒂</t>
+  </si>
+  <si>
+    <t>迈凯伦</t>
+  </si>
+  <si>
+    <t>迈巴赫</t>
+  </si>
+  <si>
+    <t>摩根</t>
+  </si>
+  <si>
+    <t>明君华凯</t>
+  </si>
+  <si>
+    <t>哪吒汽车</t>
+  </si>
+  <si>
+    <t>南京金龙</t>
+  </si>
+  <si>
+    <t>nanoFLOWCELL</t>
+  </si>
+  <si>
+    <t>Noble</t>
+  </si>
+  <si>
+    <t>NEVS国能汽车</t>
+  </si>
+  <si>
+    <t>欧拉</t>
+  </si>
+  <si>
+    <t>欧睿</t>
+  </si>
+  <si>
+    <t>欧朗</t>
+  </si>
+  <si>
+    <t>帕加尼</t>
+  </si>
+  <si>
+    <t>Polestar</t>
+  </si>
+  <si>
+    <t>前途</t>
+  </si>
+  <si>
+    <t>乔治·巴顿</t>
+  </si>
+  <si>
+    <t>庆铃汽车</t>
+  </si>
+  <si>
+    <t>瑞麒</t>
+  </si>
+  <si>
+    <t>容大智造</t>
+  </si>
+  <si>
+    <t>Rossion</t>
+  </si>
+  <si>
+    <t>赛麟</t>
+  </si>
+  <si>
+    <t>斯达泰克</t>
+  </si>
+  <si>
+    <t>世爵</t>
+  </si>
+  <si>
+    <t>SOL思皓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>泰卡特</t>
+  </si>
+  <si>
+    <t>塔塔</t>
+  </si>
+  <si>
+    <t>泰克鲁斯·腾风</t>
+  </si>
+  <si>
+    <t>威兹曼</t>
+  </si>
+  <si>
+    <t>威麟</t>
+  </si>
+  <si>
+    <t>W Motors</t>
+  </si>
+  <si>
+    <t>沃克斯豪尔</t>
+  </si>
+  <si>
+    <t>新特</t>
+  </si>
+  <si>
+    <t>延龙汽车</t>
+  </si>
+  <si>
+    <t>游侠</t>
+  </si>
+  <si>
+    <t>中兴</t>
+  </si>
+  <si>
+    <t>中欧</t>
+  </si>
+  <si>
+    <t>正道汽车</t>
+  </si>
+  <si>
+    <t>中顺</t>
+  </si>
+  <si>
+    <t>Zenvo</t>
+  </si>
+  <si>
+    <t>宾利</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -56,12 +347,6 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,8 +375,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -407,30 +692,510 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1FBA22C-B472-9A4C-837C-5D832DD17F0C}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="17">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>